<commit_message>
style: estilização da planilha
</commit_message>
<xml_diff>
--- a/Relatórios/Selection/Selection Sort (2).xlsx
+++ b/Relatórios/Selection/Selection Sort (2).xlsx
@@ -1,40 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jodes\OneDrive\Documentos\Projetos-GitHub\PAA\Relatórios\Selection\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587BABB1-DFE7-42B2-8D10-683ED28B0B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Tamanho do Vetor</t>
+  </si>
+  <si>
+    <t>Vetor Aleatório</t>
+  </si>
+  <si>
+    <t>Vetor Ordenado</t>
+  </si>
+  <si>
+    <t>Vetor Inversamente Ordenado</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -46,93 +101,56 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="3">
+    <cellStyle name="20% - Ênfase4" xfId="2" builtinId="42"/>
+    <cellStyle name="Ênfase4" xfId="1" builtinId="41"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,192 +438,188 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Tamanho do Vetor</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Vetor Aleatório</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Vetor Ordenado</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Vetor Inversamente Ordenado</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
         <v>1000</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.01660849999825587</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.02305079999860027</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.01644990000204416</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="C2" s="4">
+        <v>1.6608499998255869E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2.3050799998600269E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1.644990000204416E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="3">
         <v>5000</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.4421579000008933</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.4391847000006237</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.4107499000019743</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="C3" s="4">
+        <v>0.44215790000089328</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.43918470000062371</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.41074990000197431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="3">
         <v>10000</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="4">
         <v>1.575398800003313</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="4">
         <v>1.922295600001235</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="4">
         <v>1.598477300001832</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="3">
         <v>15000</v>
       </c>
-      <c r="C5" t="n">
-        <v>3.814865899999859</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4.383507300000929</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="C5" s="4">
+        <v>3.8148658999998588</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4.3835073000009288</v>
+      </c>
+      <c r="E5" s="4">
         <v>3.752227099997981</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="3">
         <v>20000</v>
       </c>
-      <c r="C6" t="n">
-        <v>6.87406639999972</v>
-      </c>
-      <c r="D6" t="n">
-        <v>7.280390799998713</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="C6" s="4">
+        <v>6.8740663999997196</v>
+      </c>
+      <c r="D6" s="4">
+        <v>7.2803907999987132</v>
+      </c>
+      <c r="E6" s="4">
         <v>6.552725499997905</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="3">
         <v>25000</v>
       </c>
-      <c r="C7" t="n">
-        <v>11.21250870000222</v>
-      </c>
-      <c r="D7" t="n">
-        <v>10.97075359999872</v>
-      </c>
-      <c r="E7" t="n">
-        <v>10.37994869999966</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="C7" s="4">
+        <v>11.212508700002219</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10.970753599998719</v>
+      </c>
+      <c r="E7" s="4">
+        <v>10.379948699999661</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="3">
         <v>30000</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="4">
         <v>15.99224949999916</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="4">
         <v>14.41369130000021</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="4">
         <v>15.06683260000136</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="3">
         <v>35000</v>
       </c>
-      <c r="C9" t="n">
-        <v>20.14293039999757</v>
-      </c>
-      <c r="D9" t="n">
-        <v>22.7514013</v>
-      </c>
-      <c r="E9" t="n">
-        <v>19.94302120000066</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="C9" s="4">
+        <v>20.142930399997571</v>
+      </c>
+      <c r="D9" s="4">
+        <v>22.751401300000001</v>
+      </c>
+      <c r="E9" s="4">
+        <v>19.943021200000661</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="3">
         <v>40000</v>
       </c>
-      <c r="C10" t="n">
-        <v>28.54314250000243</v>
-      </c>
-      <c r="D10" t="n">
-        <v>24.93201259999842</v>
-      </c>
-      <c r="E10" t="n">
-        <v>25.79898669999966</v>
+      <c r="C10" s="4">
+        <v>28.543142500002428</v>
+      </c>
+      <c r="D10" s="4">
+        <v>24.932012599998419</v>
+      </c>
+      <c r="E10" s="4">
+        <v>25.798986699999659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>